<commit_message>
Add clean test databases with clearly fake data patterns
</commit_message>
<xml_diff>
--- a/databases/excel/Healthcare_Records.xlsx
+++ b/databases/excel/Healthcare_Records.xlsx
@@ -523,77 +523,77 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1996-02-26</t>
+          <t>1973-06-16</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>438-92-4502</t>
+          <t>670-74-9362</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>9526 Care Dr</t>
+          <t>4157 Health Dr</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>889-330-1704</t>
+          <t>222-851-2388</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>patient.james.jackson@healthcare.org</t>
+          <t>patient.robert.thomas@healthcare.org</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Spouse: (539) 170-2160</t>
+          <t>Child: (810) 238-9181</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Diabetes</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Lisinopril</t>
+          <t>Ibuprofen</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2024-03-07</t>
+          <t>2024-06-24</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2024-10-10</t>
+          <t>2024-10-17</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>INS794127</t>
+          <t>INS360499</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>Aetna</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 3 months.</t>
         </is>
       </c>
     </row>
@@ -610,72 +610,72 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Moore</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1967-03-03</t>
+          <t>1975-11-12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>809-93-1945</t>
+          <t>633-35-9261</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>9403 Medical Dr</t>
+          <t>9531 Health Dr</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>339-238-5123</t>
+          <t>458-353-4461</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>patient.david.moore@healthcare.org</t>
+          <t>patient.david.jackson@healthcare.org</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Spouse: (319) 547-1701</t>
+          <t>Spouse: (723) 856-3236</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Migraine</t>
+          <t>Anxiety</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Albuterol</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2024-08-20</t>
+          <t>2024-05-15</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2024-03-15</t>
+          <t>2024-11-06</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>INS928499</t>
+          <t>INS348310</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>Cigna</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 6 months.</t>
         </is>
       </c>
     </row>
@@ -692,72 +692,72 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1943-04-14</t>
+          <t>1966-11-10</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>282-27-2479</t>
+          <t>627-39-3971</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>8642 Care Dr</t>
+          <t>8372 Care Dr</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>739-460-4742</t>
+          <t>932-646-4832</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>patient.james.jackson@healthcare.org</t>
+          <t>patient.james.thomas@healthcare.org</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Child: (238) 810-5740</t>
+          <t>Child: (279) 244-9856</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Arthritis</t>
+          <t>Migraine</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Metformin</t>
+          <t>Sumatriptan</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2024-01-23</t>
+          <t>2024-05-05</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2024-02-21</t>
+          <t>2024-02-12</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>INS533696</t>
+          <t>INS885170</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>Aetna</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 6 months.</t>
         </is>
       </c>
     </row>
@@ -769,47 +769,47 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Moore</t>
+          <t>White</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1997-03-28</t>
+          <t>1942-03-21</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>249-57-5696</t>
+          <t>135-98-3835</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>8217 Care Dr</t>
+          <t>8190 Wellness Dr</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>638-632-6349</t>
+          <t>201-628-2869</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>patient.elizabeth.moore@healthcare.org</t>
+          <t>patient.linda.white@healthcare.org</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Spouse: (784) 819-1125</t>
+          <t>Child: (687) 400-8497</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Migraine</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -819,17 +819,17 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2024-05-17</t>
+          <t>2024-07-08</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2024-03-21</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>INS764733</t>
+          <t>INS499205</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 3 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -861,22 +861,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1955-10-28</t>
+          <t>1946-09-25</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>607-58-6030</t>
+          <t>463-94-7501</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>187 Medical Dr</t>
+          <t>7210 Care Dr</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>455-294-6596</t>
+          <t>542-429-1628</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -886,42 +886,42 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Child: (995) 599-5427</t>
+          <t>Child: (266) 302-4217</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Ibuprofen</t>
+          <t>Atorvastatin</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2024-09-12</t>
+          <t>2024-04-16</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2024-09-15</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>INS608327</t>
+          <t>INS199710</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Aetna</t>
+          <t>Cigna</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 5 months.</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -943,32 +943,32 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1975-05-10</t>
+          <t>1990-01-07</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>469-92-5313</t>
+          <t>385-22-3842</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>9508 Medical Dr</t>
+          <t>2792 Health Dr</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>840-494-1989</t>
+          <t>903-967-3988</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>patient.susan.taylor@healthcare.org</t>
+          <t>patient.robert.taylor@healthcare.org</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Spouse: (653) 718-9948</t>
+          <t>Parent: (763) 154-5247</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -978,22 +978,22 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-01-22</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2024-05-18</t>
+          <t>2024-06-11</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>INS215918</t>
+          <t>INS160865</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 3 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 6 months.</t>
         </is>
       </c>
     </row>
@@ -1015,77 +1015,77 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Moore</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1958-08-25</t>
+          <t>1996-11-08</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>810-62-2960</t>
+          <t>642-44-2643</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>6209 Health Dr</t>
+          <t>6162 Care Dr</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>958-607-1925</t>
+          <t>683-445-3706</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>patient.patricia.moore@healthcare.org</t>
+          <t>patient.robert.wilson@healthcare.org</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Parent: (698) 390-8497</t>
+          <t>Parent: (655) 191-3972</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Ibuprofen</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-04-27</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2024-05-19</t>
+          <t>2024-03-04</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>INS589662</t>
+          <t>INS715924</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Aetna</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 6 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 2 months.</t>
         </is>
       </c>
     </row>
@@ -1097,77 +1097,77 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Susan</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>White</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1947-05-11</t>
+          <t>1947-01-11</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>515-86-6268</t>
+          <t>488-88-3088</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>243 Care Dr</t>
+          <t>999 Wellness Dr</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>593-752-5285</t>
+          <t>614-490-5878</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>patient.susan.taylor@healthcare.org</t>
+          <t>patient.elizabeth.white@healthcare.org</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Child: (575) 627-5067</t>
+          <t>Child: (760) 279-5478</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Arthritis</t>
+          <t>Anxiety</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Ibuprofen</t>
+          <t>Sertraline</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2024-02-03</t>
+          <t>2024-04-26</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2024-05-21</t>
+          <t>2024-10-25</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>INS182103</t>
+          <t>INS356404</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>Aetna</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1189,57 +1189,57 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1943-08-28</t>
+          <t>1944-06-09</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>457-99-8776</t>
+          <t>814-54-4594</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2535 Care Dr</t>
+          <t>552 Wellness Dr</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>471-759-9230</t>
+          <t>248-628-5891</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>patient.linda.thomas@healthcare.org</t>
+          <t>patient.robert.thomas@healthcare.org</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Parent: (854) 287-2436</t>
+          <t>Spouse: (310) 467-1675</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Arthritis</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Ibuprofen</t>
+          <t>Metformin</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-02-12</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2024-06-20</t>
+          <t>2024-11-21</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>INS983482</t>
+          <t>INS834029</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 1 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
         </is>
       </c>
     </row>
@@ -1261,47 +1261,47 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1990-06-12</t>
+          <t>1945-05-01</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>500-53-7245</t>
+          <t>890-42-3621</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2708 Wellness Dr</t>
+          <t>8446 Care Dr</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>261-350-8482</t>
+          <t>616-468-7353</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>patient.david.harris@healthcare.org</t>
+          <t>patient.patricia.moore@healthcare.org</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Spouse: (596) 256-3645</t>
+          <t>Spouse: (552) 650-8204</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Hypertension</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1311,27 +1311,27 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2024-05-03</t>
+          <t>2024-08-10</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2024-12-15</t>
+          <t>2024-06-27</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>INS437541</t>
+          <t>INS277541</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Aetna</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 5 months.</t>
         </is>
       </c>
     </row>
@@ -1343,77 +1343,77 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1962-03-21</t>
+          <t>1959-06-04</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>314-25-6687</t>
+          <t>241-45-9851</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3280 Wellness Dr</t>
+          <t>9172 Care Dr</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>400-660-6720</t>
+          <t>846-155-2411</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>patient.patricia.harris@healthcare.org</t>
+          <t>patient.david.anderson@healthcare.org</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Spouse: (663) 850-9629</t>
+          <t>Child: (780) 294-6059</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Migraine</t>
+          <t>Diabetes</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Albuterol</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2024-12-24</t>
+          <t>2024-06-07</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2024-05-06</t>
+          <t>2024-02-28</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>INS343016</t>
+          <t>INS153321</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>UnitedHealth</t>
+          <t>Cigna</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 3 months.</t>
         </is>
       </c>
     </row>
@@ -1425,77 +1425,77 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Robert</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1952-11-04</t>
+          <t>1965-04-26</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>246-79-1377</t>
+          <t>612-93-5585</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>6014 Health Dr</t>
+          <t>7518 Health Dr</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>219-571-4281</t>
+          <t>718-192-1343</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>patient.patricia.taylor@healthcare.org</t>
+          <t>patient.robert.thomas@healthcare.org</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Child: (777) 486-9925</t>
+          <t>Child: (635) 853-6628</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Hypertension</t>
+          <t>Migraine</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Atorvastatin</t>
+          <t>Metformin</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2024-09-15</t>
+          <t>2024-12-27</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2024-06-26</t>
+          <t>2024-02-26</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>INS416783</t>
+          <t>INS952524</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Cigna</t>
+          <t>BlueCross</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 3 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -1507,77 +1507,77 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1996-12-05</t>
+          <t>1984-02-25</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>325-35-8952</t>
+          <t>738-13-5496</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4448 Medical Dr</t>
+          <t>5212 Health Dr</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>273-104-7260</t>
+          <t>229-319-4453</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>patient.elizabeth.harris@healthcare.org</t>
+          <t>patient.james.anderson@healthcare.org</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Parent: (780) 817-4261</t>
+          <t>Child: (588) 234-4986</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Anxiety</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Sertraline</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2024-05-11</t>
+          <t>2024-04-04</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>2024-06-24</t>
+          <t>2024-02-07</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>INS204799</t>
+          <t>INS921033</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Aetna</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 1 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 5 months.</t>
         </is>
       </c>
     </row>
@@ -1589,77 +1589,77 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1952-05-14</t>
+          <t>1963-08-24</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>965-15-3865</t>
+          <t>739-99-3982</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>3275 Medical Dr</t>
+          <t>3331 Health Dr</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>454-847-1946</t>
+          <t>438-162-3195</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>patient.william.taylor@healthcare.org</t>
+          <t>patient.patricia.anderson@healthcare.org</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Child: (960) 193-6135</t>
+          <t>Parent: (780) 323-9257</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Anxiety</t>
+          <t>Arthritis</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sertraline</t>
+          <t>Metformin</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2024-04-02</t>
+          <t>2024-09-16</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2024-06-06</t>
+          <t>2024-05-14</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>INS214046</t>
+          <t>INS274762</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>UnitedHealth</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 6 months.</t>
         </is>
       </c>
     </row>
@@ -1671,77 +1671,77 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1958-05-07</t>
+          <t>1981-10-27</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>340-72-2327</t>
+          <t>337-17-7804</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1492 Care Dr</t>
+          <t>329 Care Dr</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>431-630-8399</t>
+          <t>861-568-9735</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>patient.william.wilson@healthcare.org</t>
+          <t>patient.linda.moore@healthcare.org</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Spouse: (822) 915-5730</t>
+          <t>Parent: (861) 341-8406</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Migraine</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Metformin</t>
+          <t>Atorvastatin</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2024-01-04</t>
+          <t>2024-01-21</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>2024-03-04</t>
+          <t>2024-09-10</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>INS136526</t>
+          <t>INS497591</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>UnitedHealth</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 5 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 6 months.</t>
         </is>
       </c>
     </row>
@@ -1753,77 +1753,77 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Patricia</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1987-05-04</t>
+          <t>1972-04-04</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>938-70-1017</t>
+          <t>637-43-7569</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>1368 Care Dr</t>
+          <t>6997 Wellness Dr</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>679-620-5865</t>
+          <t>336-247-3987</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>patient.patricia.anderson@healthcare.org</t>
+          <t>patient.elizabeth.taylor@healthcare.org</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Child: (207) 926-8602</t>
+          <t>Parent: (876) 623-7261</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Arthritis</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Atorvastatin</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2024-08-15</t>
+          <t>2024-09-25</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2024-05-20</t>
+          <t>2024-11-22</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>INS232601</t>
+          <t>INS652725</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>UnitedHealth</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 3 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -1835,72 +1835,72 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Linda</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1993-02-02</t>
+          <t>1985-09-21</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>597-96-1328</t>
+          <t>982-30-1979</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>4262 Medical Dr</t>
+          <t>3411 Medical Dr</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>463-852-9379</t>
+          <t>440-413-6344</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>patient.linda.harris@healthcare.org</t>
+          <t>patient.william.anderson@healthcare.org</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Child: (738) 577-6134</t>
+          <t>Child: (788) 212-4296</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Anxiety</t>
+          <t>Migraine</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Atorvastatin</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2024-12-20</t>
+          <t>2024-12-09</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>2024-02-04</t>
+          <t>2024-01-07</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>INS124387</t>
+          <t>INS160665</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1917,77 +1917,77 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1971-02-08</t>
+          <t>1952-12-28</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>811-30-7254</t>
+          <t>571-12-7991</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4454 Medical Dr</t>
+          <t>3004 Medical Dr</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>638-694-7433</t>
+          <t>731-128-4642</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>patient.james.jackson@healthcare.org</t>
+          <t>patient.william.moore@healthcare.org</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Child: (942) 555-5971</t>
+          <t>Parent: (829) 322-8843</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Migraine</t>
+          <t>Arthritis</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Metformin</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>2024-10-03</t>
+          <t>2024-04-08</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2024-12-26</t>
+          <t>2024-10-27</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>INS482823</t>
+          <t>INS353279</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>UnitedHealth</t>
+          <t>Cigna</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 5 months.</t>
         </is>
       </c>
     </row>
@@ -1999,42 +1999,42 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Harris</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1972-11-19</t>
+          <t>1958-01-24</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>371-26-9630</t>
+          <t>142-26-5970</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>3635 Care Dr</t>
+          <t>9448 Care Dr</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>640-806-1226</t>
+          <t>416-159-1817</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>patient.william.jackson@healthcare.org</t>
+          <t>patient.elizabeth.harris@healthcare.org</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Child: (465) 585-3368</t>
+          <t>Spouse: (556) 228-3000</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2049,27 +2049,27 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>2024-08-24</t>
+          <t>2024-08-04</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>2024-12-07</t>
+          <t>2024-07-07</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>INS495015</t>
+          <t>INS547013</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Humana</t>
+          <t>Cigna</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 6 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>William</t>
+          <t>Patricia</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -2091,67 +2091,67 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1949-04-01</t>
+          <t>1962-03-20</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>318-11-1308</t>
+          <t>723-76-9965</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>4027 Care Dr</t>
+          <t>6338 Medical Dr</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>456-967-1416</t>
+          <t>462-785-4154</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>patient.william.wilson@healthcare.org</t>
+          <t>patient.patricia.wilson@healthcare.org</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Spouse: (429) 691-4750</t>
+          <t>Spouse: (284) 629-6168</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Arthritis</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Ibuprofen</t>
+          <t>Sumatriptan</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-09-04</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2024-07-17</t>
+          <t>2024-11-28</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>INS261156</t>
+          <t>INS953214</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Humana</t>
+          <t>Aetna</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 4 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 2 months.</t>
         </is>
       </c>
     </row>
@@ -2163,77 +2163,77 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1941-07-01</t>
+          <t>1961-09-07</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>698-59-8234</t>
+          <t>565-47-9828</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>951 Care Dr</t>
+          <t>3176 Health Dr</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>985-311-9582</t>
+          <t>910-981-1286</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>patient.david.harris@healthcare.org</t>
+          <t>patient.elizabeth.wilson@healthcare.org</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Child: (251) 257-7077</t>
+          <t>Parent: (389) 496-6980</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Anxiety</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Sertraline</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2024-02-08</t>
+          <t>2024-12-26</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2024-04-10</t>
+          <t>2024-08-21</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>INS876160</t>
+          <t>INS353985</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>UnitedHealth</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 1 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -2245,77 +2245,77 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1975-12-24</t>
+          <t>1981-12-13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>891-14-4859</t>
+          <t>344-27-2312</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>7010 Wellness Dr</t>
+          <t>9825 Health Dr</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>662-110-6507</t>
+          <t>901-262-4301</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>patient.elizabeth.anderson@healthcare.org</t>
+          <t>patient.susan.wilson@healthcare.org</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Spouse: (745) 171-4502</t>
+          <t>Spouse: (441) 628-3566</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Diabetes</t>
+          <t>Asthma</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Ibuprofen</t>
+          <t>Metformin</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>2024-08-11</t>
+          <t>2024-12-05</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>2024-08-27</t>
+          <t>2024-02-18</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>INS636684</t>
+          <t>INS136337</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Aetna</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 6 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -2327,77 +2327,77 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Wilson</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>1944-03-20</t>
+          <t>1955-01-02</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>491-56-7493</t>
+          <t>394-18-4673</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>5307 Wellness Dr</t>
+          <t>8655 Health Dr</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>599-937-4880</t>
+          <t>906-261-1280</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>patient.elizabeth.wilson@healthcare.org</t>
+          <t>patient.james.jackson@healthcare.org</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Child: (855) 995-9988</t>
+          <t>Spouse: (963) 764-7310</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Hypertension</t>
+          <t>Depression</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Albuterol</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>2024-11-18</t>
+          <t>2024-07-03</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>2024-03-13</t>
+          <t>2024-03-15</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>INS138928</t>
+          <t>INS705366</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>UnitedHealth</t>
+          <t>Cigna</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 5 months.</t>
         </is>
       </c>
     </row>
@@ -2409,77 +2409,77 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>James</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1971-01-17</t>
+          <t>1964-07-26</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>687-34-7306</t>
+          <t>185-69-8606</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>270 Health Dr</t>
+          <t>6559 Health Dr</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>600-344-7406</t>
+          <t>513-309-4990</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>patient.robert.anderson@healthcare.org</t>
+          <t>patient.james.taylor@healthcare.org</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Spouse: (323) 181-3313</t>
+          <t>Parent: (388) 384-1009</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Migraine</t>
+          <t>Anxiety</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Lisinopril</t>
+          <t>Metformin</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2024-05-20</t>
+          <t>2024-09-18</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>2024-12-08</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>INS938255</t>
+          <t>INS274481</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Cigna</t>
+          <t>Humana</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 5 months.</t>
         </is>
       </c>
     </row>
@@ -2491,67 +2491,67 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1996-02-24</t>
+          <t>1955-10-16</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>884-96-9895</t>
+          <t>990-74-8748</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2611 Health Dr</t>
+          <t>4968 Wellness Dr</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>392-863-2484</t>
+          <t>910-815-6755</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>patient.david.harris@healthcare.org</t>
+          <t>patient.susan.jackson@healthcare.org</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Spouse: (538) 162-3781</t>
+          <t>Spouse: (963) 294-2444</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Arthritis</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Atorvastatin</t>
+          <t>Sertraline</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2024-02-02</t>
+          <t>2024-08-15</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>2024-01-15</t>
+          <t>2024-08-13</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>INS375365</t>
+          <t>INS333543</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 2 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 1 months.</t>
         </is>
       </c>
     </row>
@@ -2573,47 +2573,47 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Elizabeth</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1948-07-16</t>
+          <t>1962-03-03</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>826-10-4598</t>
+          <t>573-29-9529</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2330 Care Dr</t>
+          <t>6676 Wellness Dr</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>920-715-9892</t>
+          <t>521-834-8354</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>patient.david.thomas@healthcare.org</t>
+          <t>patient.elizabeth.taylor@healthcare.org</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Child: (492) 946-7187</t>
+          <t>Spouse: (213) 978-6989</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2623,27 +2623,27 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2024-07-07</t>
+          <t>2024-08-10</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>2024-08-18</t>
+          <t>2024-12-02</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>INS488802</t>
+          <t>INS783960</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Humana</t>
+          <t>UnitedHealth</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 3 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 2 months.</t>
         </is>
       </c>
     </row>
@@ -2660,72 +2660,72 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1991-10-19</t>
+          <t>1958-10-17</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>736-55-1589</t>
+          <t>769-42-8332</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>4184 Wellness Dr</t>
+          <t>3680 Wellness Dr</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>261-680-3547</t>
+          <t>608-268-2430</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>patient.robert.white@healthcare.org</t>
+          <t>patient.robert.thomas@healthcare.org</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Parent: (814) 400-3672</t>
+          <t>Parent: (527) 271-6785</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Hypertension</t>
+          <t>Arthritis</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Albuterol</t>
+          <t>Sumatriptan</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2024-07-27</t>
+          <t>2024-08-07</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>2024-07-05</t>
+          <t>2024-07-13</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>INS874544</t>
+          <t>INS251056</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Humana</t>
+          <t>BlueCross</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 3 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 2 months.</t>
         </is>
       </c>
     </row>
@@ -2737,77 +2737,77 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Susan</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1959-10-14</t>
+          <t>1951-12-16</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>155-21-5723</t>
+          <t>168-31-3975</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1595 Health Dr</t>
+          <t>261 Health Dr</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>420-845-5820</t>
+          <t>818-501-2616</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>patient.david.white@healthcare.org</t>
+          <t>patient.susan.thomas@healthcare.org</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Child: (583) 748-8420</t>
+          <t>Parent: (938) 421-8873</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Anxiety</t>
+          <t>Hypertension</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sumatriptan</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2024-09-19</t>
+          <t>2024-09-20</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>2024-08-22</t>
+          <t>2024-02-26</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>INS421853</t>
+          <t>INS255318</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Cigna</t>
+          <t>UnitedHealth</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Patient presents with mild symptoms. Follow up in 5 months.</t>
+          <t>Patient presents with mild symptoms. Follow up in 4 months.</t>
         </is>
       </c>
     </row>
@@ -2819,77 +2819,77 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Robert</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Harris</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1979-05-10</t>
+          <t>1954-06-26</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>916-62-5058</t>
+          <t>185-64-1683</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>7770 Health Dr</t>
+          <t>5345 Wellness Dr</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>475-497-4349</t>
+          <t>325-417-9099</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>patient.robert.jackson@healthcare.org</t>
+          <t>patient.linda.harris@healthcare.org</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Spouse: (869) 415-8706</t>
+          <t>Child: (629) 843-6869</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Diabetes</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Lisinopril</t>
+          <t>Albuterol</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>2024-11-19</t>
+          <t>2024-12-28</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>2024-08-19</t>
+          <t>2024-04-27</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>INS566971</t>
+          <t>INS920275</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>BlueCross</t>
+          <t>Aetna</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Patient presents with moderate symptoms. Follow up in 1 months.</t>
+          <t>Patient presents with severe symptoms. Follow up in 2 months.</t>
         </is>
       </c>
     </row>
@@ -2901,77 +2901,77 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Elizabeth</t>
+          <t>David</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Moore</t>
+          <t>White</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1961-12-02</t>
+          <t>1940-11-02</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>655-89-1247</t>
+          <t>291-14-7766</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>6152 Medical Dr</t>
+          <t>2003 Medical Dr</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>688-397-6449</t>
+          <t>744-670-8479</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>patient.elizabeth.moore@healthcare.org</t>
+          <t>patient.david.white@healthcare.org</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Parent: (646) 191-4314</t>
+          <t>Child: (948) 873-9731</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Depression</t>
+          <t>Anxiety</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Metformin</t>
+          <t>Lisinopril</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2024-07-12</t>
+          <t>2024-08-24</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>2024-01-28</t>
+          <t>2024-12-17</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>INS868173</t>
+          <t>INS801792</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Cigna</t>
+          <t>UnitedHealth</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Patient presents with severe symptoms. Follow up in 5 months.</t>
+          <t>Patient presents with moderate symptoms. Follow up in 2 months.</t>
         </is>
       </c>
     </row>

</xml_diff>